<commit_message>
10th Commit | Important Commit
- Added NASS data for year 2022. Now the model have 6 census years
- Added winter rye
- Fertilizer use is based on NASS Ag. Chemical use
- Changed import_yrs to year_labels.
- Fixed population values for 2012, 2017
- CMAQ data added
</commit_message>
<xml_diff>
--- a/RawData/animdatadyn_master.xlsx
+++ b/RawData/animdatadyn_master.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/lds5498_psu_edu/Documents/CSNAPNI/CSNAPNI/CBW-CSNAPNI/CB_CSNAPNI/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_E30DB14B9EDAFFA1F00858210F051D885B68AE5C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3CAA9CC-A477-403E-8C80-89E4B249A017}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_E30DB14B9EDAFFA1F00858210F051D885B68AE5C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{095B91CA-B4C3-4DEE-B217-6C52CA61684D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animdatadyn_master" sheetId="1" r:id="rId1"/>
-    <sheet name="animdatadyn" sheetId="2" r:id="rId2"/>
-    <sheet name="animdatadyn_key" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="animdatadyn" sheetId="2" r:id="rId3"/>
+    <sheet name="animdatadyn_key" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
   <si>
     <t>Type</t>
   </si>
@@ -229,7 +230,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,8 +257,14 @@
         <fgColor rgb="FFF8CBAD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -287,11 +294,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -419,6 +446,54 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,15 +801,15 @@
   </sheetPr>
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K11"/>
+    <sheetView topLeftCell="O9" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" style="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="11" style="41" hidden="1" customWidth="1"/>
+    <col min="3" max="9" width="11" style="41" customWidth="1"/>
     <col min="10" max="10" width="11" style="42" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1796875" style="43" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="41" bestFit="1" customWidth="1"/>
@@ -3231,6 +3306,723 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FB9E45-30CA-4FC2-ADDE-E4F683EE8F2A}">
+  <dimension ref="B2:L21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" ht="87" x14ac:dyDescent="0.35">
+      <c r="B2" s="45"/>
+      <c r="C2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="52">
+        <v>1</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="51">
+        <v>50.3</v>
+      </c>
+      <c r="E3" s="52">
+        <v>48</v>
+      </c>
+      <c r="F3" s="51">
+        <v>19.2</v>
+      </c>
+      <c r="G3" s="52">
+        <v>10</v>
+      </c>
+      <c r="H3" s="53">
+        <v>463</v>
+      </c>
+      <c r="I3" s="54">
+        <v>0.42200000000000004</v>
+      </c>
+      <c r="J3" s="54">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K3" s="53">
+        <v>2910</v>
+      </c>
+      <c r="L3" s="54">
+        <v>173.2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="52">
+        <v>2</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="51">
+        <v>233.85</v>
+      </c>
+      <c r="E4" s="52">
+        <v>150.63</v>
+      </c>
+      <c r="F4" s="52">
+        <v>26</v>
+      </c>
+      <c r="G4" s="52">
+        <v>10</v>
+      </c>
+      <c r="H4" s="53">
+        <v>10068.67</v>
+      </c>
+      <c r="I4" s="53">
+        <v>1</v>
+      </c>
+      <c r="J4" s="54">
+        <v>4.96E-3</v>
+      </c>
+      <c r="K4" s="53">
+        <v>610</v>
+      </c>
+      <c r="L4" s="54">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="52">
+        <v>3</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="51">
+        <v>13.8</v>
+      </c>
+      <c r="E5" s="51">
+        <v>9.1</v>
+      </c>
+      <c r="F5" s="51">
+        <v>4.7</v>
+      </c>
+      <c r="G5" s="52">
+        <v>10</v>
+      </c>
+      <c r="H5" s="53">
+        <v>0</v>
+      </c>
+      <c r="I5" s="53">
+        <v>0</v>
+      </c>
+      <c r="J5" s="53">
+        <v>0</v>
+      </c>
+      <c r="K5" s="53">
+        <v>0</v>
+      </c>
+      <c r="L5" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="52">
+        <v>4</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="52">
+        <v>24</v>
+      </c>
+      <c r="E6" s="51">
+        <v>5.8</v>
+      </c>
+      <c r="F6" s="52">
+        <v>3</v>
+      </c>
+      <c r="G6" s="52">
+        <v>10</v>
+      </c>
+      <c r="H6" s="53">
+        <v>112</v>
+      </c>
+      <c r="I6" s="54">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="J6" s="54">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="K6" s="53">
+        <v>4720</v>
+      </c>
+      <c r="L6" s="54">
+        <v>139.19999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="52">
+        <v>5</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="51">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="51">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="51">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="52">
+        <v>10</v>
+      </c>
+      <c r="H7" s="54">
+        <v>14.5</v>
+      </c>
+      <c r="I7" s="54">
+        <v>0.89</v>
+      </c>
+      <c r="J7" s="54">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="K7" s="53">
+        <v>1430</v>
+      </c>
+      <c r="L7" s="54">
+        <v>125.60000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="52">
+        <v>6</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="51">
+        <v>2.1</v>
+      </c>
+      <c r="E8" s="51">
+        <v>1.7</v>
+      </c>
+      <c r="F8" s="51">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="52">
+        <v>10</v>
+      </c>
+      <c r="H8" s="53">
+        <v>0</v>
+      </c>
+      <c r="I8" s="53">
+        <v>0</v>
+      </c>
+      <c r="J8" s="53">
+        <v>0</v>
+      </c>
+      <c r="K8" s="53">
+        <v>0</v>
+      </c>
+      <c r="L8" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="52">
+        <v>7</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="51">
+        <v>0.4</v>
+      </c>
+      <c r="E9" s="51">
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="51">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="52">
+        <v>10</v>
+      </c>
+      <c r="H9" s="53">
+        <v>0</v>
+      </c>
+      <c r="I9" s="53">
+        <v>0</v>
+      </c>
+      <c r="J9" s="53">
+        <v>0</v>
+      </c>
+      <c r="K9" s="53">
+        <v>0</v>
+      </c>
+      <c r="L9" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="52">
+        <v>8</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="51">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="51">
+        <v>0.7</v>
+      </c>
+      <c r="F10" s="51">
+        <v>0.3</v>
+      </c>
+      <c r="G10" s="52">
+        <v>10</v>
+      </c>
+      <c r="H10" s="54">
+        <v>1.71</v>
+      </c>
+      <c r="I10" s="54">
+        <v>0.69</v>
+      </c>
+      <c r="J10" s="54">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="K10" s="53">
+        <v>2130</v>
+      </c>
+      <c r="L10" s="54">
+        <v>183.29999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="52">
+        <v>9</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="51">
+        <v>2.1</v>
+      </c>
+      <c r="E11" s="51">
+        <v>1.6</v>
+      </c>
+      <c r="F11" s="51">
+        <v>0.7</v>
+      </c>
+      <c r="G11" s="52">
+        <v>10</v>
+      </c>
+      <c r="H11" s="54">
+        <v>8.51</v>
+      </c>
+      <c r="I11" s="54">
+        <v>0.79</v>
+      </c>
+      <c r="J11" s="54">
+        <v>2.9300000000000003E-2</v>
+      </c>
+      <c r="K11" s="53">
+        <v>1570</v>
+      </c>
+      <c r="L11" s="54">
+        <v>203.70000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="52">
+        <v>10</v>
+      </c>
+      <c r="C12" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="51">
+        <v>60.9</v>
+      </c>
+      <c r="E12" s="51">
+        <v>59.8</v>
+      </c>
+      <c r="F12" s="51">
+        <v>4.8</v>
+      </c>
+      <c r="G12" s="52">
+        <v>10</v>
+      </c>
+      <c r="H12" s="53">
+        <v>0</v>
+      </c>
+      <c r="I12" s="53">
+        <v>0</v>
+      </c>
+      <c r="J12" s="53">
+        <v>0</v>
+      </c>
+      <c r="K12" s="53">
+        <v>0</v>
+      </c>
+      <c r="L12" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="52">
+        <v>11</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="51">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E13" s="51">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F13" s="51">
+        <v>0.8</v>
+      </c>
+      <c r="G13" s="52">
+        <v>10</v>
+      </c>
+      <c r="H13" s="53">
+        <v>0</v>
+      </c>
+      <c r="I13" s="53">
+        <v>0</v>
+      </c>
+      <c r="J13" s="53">
+        <v>0</v>
+      </c>
+      <c r="K13" s="53">
+        <v>0</v>
+      </c>
+      <c r="L13" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="52">
+        <v>12</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="51">
+        <v>10.6</v>
+      </c>
+      <c r="E14" s="51">
+        <v>6.7</v>
+      </c>
+      <c r="F14" s="51">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="52">
+        <v>10</v>
+      </c>
+      <c r="H14" s="53">
+        <v>0</v>
+      </c>
+      <c r="I14" s="53">
+        <v>0</v>
+      </c>
+      <c r="J14" s="53">
+        <v>0</v>
+      </c>
+      <c r="K14" s="53">
+        <v>0</v>
+      </c>
+      <c r="L14" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="52">
+        <v>13</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="51">
+        <v>40.5</v>
+      </c>
+      <c r="E15" s="51">
+        <v>28.2</v>
+      </c>
+      <c r="F15" s="51">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G15" s="52">
+        <v>10</v>
+      </c>
+      <c r="H15" s="53">
+        <v>0</v>
+      </c>
+      <c r="I15" s="53">
+        <v>0</v>
+      </c>
+      <c r="J15" s="53">
+        <v>0</v>
+      </c>
+      <c r="K15" s="53">
+        <v>0</v>
+      </c>
+      <c r="L15" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B16" s="52">
+        <v>14</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="51">
+        <v>43.5</v>
+      </c>
+      <c r="E16" s="51">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="F16" s="51">
+        <v>2.7</v>
+      </c>
+      <c r="G16" s="52">
+        <v>10</v>
+      </c>
+      <c r="H16" s="53">
+        <v>0</v>
+      </c>
+      <c r="I16" s="53">
+        <v>0</v>
+      </c>
+      <c r="J16" s="53">
+        <v>0</v>
+      </c>
+      <c r="K16" s="53">
+        <v>0</v>
+      </c>
+      <c r="L16" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="52">
+        <v>15</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="51">
+        <v>37.6</v>
+      </c>
+      <c r="E17" s="51">
+        <v>26.6</v>
+      </c>
+      <c r="F17" s="51">
+        <v>10.6</v>
+      </c>
+      <c r="G17" s="52">
+        <v>10</v>
+      </c>
+      <c r="H17" s="53">
+        <v>0</v>
+      </c>
+      <c r="I17" s="53">
+        <v>0</v>
+      </c>
+      <c r="J17" s="53">
+        <v>0</v>
+      </c>
+      <c r="K17" s="53">
+        <v>0</v>
+      </c>
+      <c r="L17" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B18" s="52">
+        <v>16</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="51">
+        <v>37.6</v>
+      </c>
+      <c r="E18" s="51">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="F18" s="51">
+        <v>7.4</v>
+      </c>
+      <c r="G18" s="52">
+        <v>10</v>
+      </c>
+      <c r="H18" s="53">
+        <v>0</v>
+      </c>
+      <c r="I18" s="53">
+        <v>0</v>
+      </c>
+      <c r="J18" s="53">
+        <v>0</v>
+      </c>
+      <c r="K18" s="53">
+        <v>0</v>
+      </c>
+      <c r="L18" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="52">
+        <v>17</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="51">
+        <v>14.5</v>
+      </c>
+      <c r="E19" s="51">
+        <v>8.4</v>
+      </c>
+      <c r="F19" s="51">
+        <v>5.6</v>
+      </c>
+      <c r="G19" s="52">
+        <v>10</v>
+      </c>
+      <c r="H19" s="54">
+        <v>44.6</v>
+      </c>
+      <c r="I19" s="54">
+        <v>0.498</v>
+      </c>
+      <c r="J19" s="54">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="K19" s="53">
+        <v>2670</v>
+      </c>
+      <c r="L19" s="54">
+        <v>168.79999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="52">
+        <v>18</v>
+      </c>
+      <c r="C20" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="51">
+        <v>44.8</v>
+      </c>
+      <c r="E20" s="52">
+        <v>40</v>
+      </c>
+      <c r="F20" s="51">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G20" s="52">
+        <v>10</v>
+      </c>
+      <c r="H20" s="53">
+        <v>0</v>
+      </c>
+      <c r="I20" s="53">
+        <v>0</v>
+      </c>
+      <c r="J20" s="53">
+        <v>0</v>
+      </c>
+      <c r="K20" s="53">
+        <v>0</v>
+      </c>
+      <c r="L20" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="56">
+        <v>19</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="55">
+        <v>5.97</v>
+      </c>
+      <c r="E21" s="56">
+        <v>5</v>
+      </c>
+      <c r="F21" s="55">
+        <v>5.26</v>
+      </c>
+      <c r="G21" s="56">
+        <v>10</v>
+      </c>
+      <c r="H21" s="57">
+        <v>45.454545454545453</v>
+      </c>
+      <c r="I21" s="57">
+        <v>0.498</v>
+      </c>
+      <c r="J21" s="57">
+        <v>3.296052948641745E-2</v>
+      </c>
+      <c r="K21" s="58">
+        <v>1090</v>
+      </c>
+      <c r="L21" s="58">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -4633,14 +5425,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4650,7 +5442,7 @@
     <col min="21" max="24" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>